<commit_message>
Added Test Data utils and models
</commit_message>
<xml_diff>
--- a/src/main/java/com/sandboxx/dataManagement/testData/test_data.xlsx
+++ b/src/main/java/com/sandboxx/dataManagement/testData/test_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -122,6 +122,170 @@
   </si>
   <si>
     <t>3452352344</t>
+  </si>
+  <si>
+    <t>registerWithEmail_AutoConnectedKin</t>
+  </si>
+  <si>
+    <t>Temp1234</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>jdoe1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>4057704109</t>
+  </si>
+  <si>
+    <t>loginWithPhoneFail</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>rsykes1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Remi</t>
+  </si>
+  <si>
+    <t>Sykes</t>
+  </si>
+  <si>
+    <t>4328940918</t>
+  </si>
+  <si>
+    <t>logOutSuccess</t>
+  </si>
+  <si>
+    <t>registerWithEmail_ExistingEmail</t>
+  </si>
+  <si>
+    <t>registerWithEmail_PhoneInUse</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>ihunter1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Isabella</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>3084999708</t>
+  </si>
+  <si>
+    <t>registerAccount_ByEmail</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>cgonzales1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Cole</t>
+  </si>
+  <si>
+    <t>Gonzales</t>
+  </si>
+  <si>
+    <t>8503308287</t>
+  </si>
+  <si>
+    <t>loginWithEmail</t>
+  </si>
+  <si>
+    <t>registerWithEmail_AddContactFromSettings</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>dkelly1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>2245061113</t>
+  </si>
+  <si>
+    <t>deleteAccountByEmail</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>rarnold1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Rosie</t>
+  </si>
+  <si>
+    <t>Arnold</t>
+  </si>
+  <si>
+    <t>4804563386</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>twidel1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Wide</t>
+  </si>
+  <si>
+    <t>2197904195</t>
   </si>
 </sst>
 </file>
@@ -339,13 +503,13 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1432,13 +1596,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="8" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.6016" style="1" customWidth="1"/>
+    <col min="2" max="3" width="16.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5078" style="1" customWidth="1"/>
+    <col min="5" max="8" width="16.3516" style="1" customWidth="1"/>
     <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1541,190 +1708,369 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="A5" t="s" s="6">
+        <v>29</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s" s="8">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s" s="8">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s" s="8">
+        <v>32</v>
+      </c>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="A6" t="s" s="6">
+        <v>33</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s" s="8">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s" s="8">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s" s="8">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s" s="8">
+        <v>37</v>
+      </c>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="A7" t="s" s="6">
+        <v>38</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s" s="8">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s" s="8">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s" s="8">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s" s="8">
+        <v>37</v>
+      </c>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="A8" t="s" s="6">
+        <v>39</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s" s="8">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s" s="8">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s" s="8">
+        <v>32</v>
+      </c>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="A9" t="s" s="6">
+        <v>40</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s" s="8">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s" s="8">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s" s="8">
+        <v>43</v>
+      </c>
+      <c r="G9" t="s" s="8">
+        <v>44</v>
+      </c>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="A10" t="s" s="6">
+        <v>45</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s" s="8">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s" s="8">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s" s="8">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s" s="8">
+        <v>49</v>
+      </c>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="A11" t="s" s="6">
+        <v>50</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s" s="8">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s" s="8">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s" s="8">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s" s="8">
+        <v>37</v>
+      </c>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+      <c r="A12" t="s" s="6">
+        <v>51</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s" s="8">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s" s="8">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s" s="8">
+        <v>54</v>
+      </c>
+      <c r="G12" t="s" s="8">
+        <v>55</v>
+      </c>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="A13" t="s" s="6">
+        <v>56</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s" s="8">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s" s="8">
+        <v>58</v>
+      </c>
+      <c r="F13" t="s" s="8">
+        <v>59</v>
+      </c>
+      <c r="G13" t="s" s="8">
+        <v>60</v>
+      </c>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="9"/>
+      <c r="C16" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s" s="8">
+        <v>61</v>
+      </c>
+      <c r="E16" t="s" s="8">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s" s="8">
+        <v>63</v>
+      </c>
+      <c r="G16" t="s" s="8">
+        <v>64</v>
+      </c>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="9"/>
+      <c r="C17" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s" s="8">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s" s="8">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s" s="8">
+        <v>54</v>
+      </c>
+      <c r="G17" t="s" s="8">
+        <v>55</v>
+      </c>
+      <c r="H17" s="10"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" ht="20.05" customHeight="1">
+      <c r="A23" s="11"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" ht="20.05" customHeight="1">
+      <c r="A24" s="11"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" ht="20.05" customHeight="1">
+      <c r="A25" s="11"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" ht="20.05" customHeight="1">
+      <c r="A26" s="11"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" location="" tooltip="" display="myemail@mail.com"/>
     <hyperlink ref="D3" r:id="rId2" location="" tooltip="" display="myemail2@mail.com"/>
     <hyperlink ref="D4" r:id="rId3" location="" tooltip="" display="myemail3@mail.com"/>
+    <hyperlink ref="D5" r:id="rId4" location="" tooltip="" display="jdoe1234@mail.com"/>
+    <hyperlink ref="D6" r:id="rId5" location="" tooltip="" display="rsykes1234@mail.com"/>
+    <hyperlink ref="D7" r:id="rId6" location="" tooltip="" display="rsykes1234@mail.com"/>
+    <hyperlink ref="D8" r:id="rId7" location="" tooltip="" display="jdoe1234@mail.com"/>
+    <hyperlink ref="D9" r:id="rId8" location="" tooltip="" display="ihunter1234@mail.com"/>
+    <hyperlink ref="D10" r:id="rId9" location="" tooltip="" display="cgonzales1234@mail.com"/>
+    <hyperlink ref="D11" r:id="rId10" location="" tooltip="" display="rsykes1234@mail.com"/>
+    <hyperlink ref="D12" r:id="rId11" location="" tooltip="" display="dkelly1234@mail.com"/>
+    <hyperlink ref="D13" r:id="rId12" location="" tooltip="" display="rarnold1234@mail.com"/>
+    <hyperlink ref="D16" r:id="rId13" location="" tooltip="" display="twidel1234@mail.com"/>
+    <hyperlink ref="D17" r:id="rId14" location="" tooltip="" display="dkelly1234@mail.com"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Added google registration tests
</commit_message>
<xml_diff>
--- a/src/main/java/com/sandboxx/dataManagement/testData/test_data.xlsx
+++ b/src/main/java/com/sandboxx/dataManagement/testData/test_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -147,6 +147,9 @@
     <t>loginWithPhoneFail</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <u val="single"/>
@@ -268,6 +271,110 @@
     <t>4804563386</t>
   </si>
   <si>
+    <t>registerWithEmail_LetterTutorial_App</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>mwalters1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Mariam</t>
+  </si>
+  <si>
+    <t>Walters</t>
+  </si>
+  <si>
+    <t>2173703531</t>
+  </si>
+  <si>
+    <t>registerWithFacebook_AutoConnectedKin</t>
+  </si>
+  <si>
+    <t>Temp@1234</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>TestSanboxx12@outlook.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Kamal</t>
+  </si>
+  <si>
+    <t>Bowman</t>
+  </si>
+  <si>
+    <t>5095852527</t>
+  </si>
+  <si>
+    <t>registerWithGoogle_AutoConnectedKin</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>lukehatfield721@gmail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Luke</t>
+  </si>
+  <si>
+    <t>Hatfield</t>
+  </si>
+  <si>
+    <t>4306941978</t>
+  </si>
+  <si>
+    <t>5/5/1985</t>
+  </si>
+  <si>
+    <t>registerWithGoogle_FamilyFriend_UnknownTrainingBase</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>rossvance247@gmail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Ross</t>
+  </si>
+  <si>
+    <t>Vance</t>
+  </si>
+  <si>
+    <t>5153164175</t>
+  </si>
+  <si>
+    <t>2/4/1995</t>
+  </si>
+  <si>
+    <t>registerWithGoogle_SendLetter</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <u val="single"/>
@@ -287,13 +394,63 @@
   <si>
     <t>2197904195</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>jkim1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Jessie</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>6105965484</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>rstone820@yahoo.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Rio</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>7542557479</t>
+  </si>
+  <si>
+    <t>3087945347</t>
+  </si>
+  <si>
+    <t>4436225915</t>
+  </si>
+  <si>
+    <t>5078431339</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -475,7 +632,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -510,6 +667,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1596,15 +1756,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="37.6016" style="1" customWidth="1"/>
+    <col min="1" max="1" width="47.6875" style="1" customWidth="1"/>
     <col min="2" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5078" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.8438" style="1" customWidth="1"/>
     <col min="5" max="8" width="16.3516" style="1" customWidth="1"/>
     <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
@@ -1733,49 +1893,51 @@
       <c r="A6" t="s" s="6">
         <v>33</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" t="s" s="7">
+        <v>34</v>
+      </c>
       <c r="C6" t="s" s="8">
         <v>30</v>
       </c>
       <c r="D6" t="s" s="8">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s" s="8">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s" s="8">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s" s="8">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H6" s="10"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="6">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" t="s" s="8">
         <v>30</v>
       </c>
       <c r="D7" t="s" s="8">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s" s="8">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s" s="8">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s" s="8">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H7" s="10"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="6">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" t="s" s="8">
@@ -1797,182 +1959,230 @@
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="6">
-        <v>40</v>
-      </c>
-      <c r="B9" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="B9" t="s" s="7">
+        <v>34</v>
+      </c>
       <c r="C9" t="s" s="8">
         <v>30</v>
       </c>
       <c r="D9" t="s" s="8">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s" s="8">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s" s="8">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G9" t="s" s="8">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="6">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" t="s" s="8">
         <v>30</v>
       </c>
       <c r="D10" t="s" s="8">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s" s="8">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s" s="8">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G10" t="s" s="8">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="6">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" t="s" s="8">
         <v>30</v>
       </c>
       <c r="D11" t="s" s="8">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s" s="8">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s" s="8">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s" s="8">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H11" s="10"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="6">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" t="s" s="8">
         <v>30</v>
       </c>
       <c r="D12" t="s" s="8">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s" s="8">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F12" t="s" s="8">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s" s="8">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H12" s="10"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="6">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" t="s" s="8">
         <v>30</v>
       </c>
       <c r="D13" t="s" s="8">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s" s="8">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s" s="8">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s" s="8">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H13" s="10"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="11"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="A14" t="s" s="6">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s" s="8">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s" s="8">
+        <v>64</v>
+      </c>
+      <c r="F14" t="s" s="8">
+        <v>65</v>
+      </c>
+      <c r="G14" t="s" s="8">
+        <v>66</v>
+      </c>
       <c r="H14" s="10"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="11"/>
+      <c r="A15" t="s" s="6">
+        <v>67</v>
+      </c>
       <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="C15" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s" s="8">
+        <v>69</v>
+      </c>
+      <c r="E15" t="s" s="8">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="G15" t="s" s="8">
+        <v>72</v>
+      </c>
       <c r="H15" s="10"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="11"/>
+      <c r="A16" t="s" s="6">
+        <v>73</v>
+      </c>
       <c r="B16" s="9"/>
       <c r="C16" t="s" s="8">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s" s="8">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s" s="8">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="F16" t="s" s="8">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="G16" t="s" s="8">
-        <v>64</v>
-      </c>
-      <c r="H16" s="10"/>
+        <v>77</v>
+      </c>
+      <c r="H16" t="s" s="8">
+        <v>78</v>
+      </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="11"/>
+      <c r="A17" t="s" s="6">
+        <v>79</v>
+      </c>
       <c r="B17" s="9"/>
       <c r="C17" t="s" s="8">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s" s="8">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s" s="8">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="F17" t="s" s="8">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="G17" t="s" s="8">
-        <v>55</v>
-      </c>
-      <c r="H17" s="10"/>
+        <v>83</v>
+      </c>
+      <c r="H17" t="s" s="8">
+        <v>84</v>
+      </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="11"/>
+      <c r="A18" t="s" s="6">
+        <v>85</v>
+      </c>
       <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
+      <c r="C18" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s" s="8">
+        <v>80</v>
+      </c>
+      <c r="E18" t="s" s="8">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s" s="8">
+        <v>82</v>
+      </c>
+      <c r="G18" t="s" s="8">
+        <v>83</v>
+      </c>
       <c r="H18" s="10"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
@@ -2008,52 +2218,180 @@
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" s="11"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
+      <c r="C22" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s" s="8">
+        <v>86</v>
+      </c>
+      <c r="E22" t="s" s="8">
+        <v>87</v>
+      </c>
+      <c r="F22" t="s" s="8">
+        <v>88</v>
+      </c>
+      <c r="G22" t="s" s="8">
+        <v>89</v>
+      </c>
       <c r="H22" s="10"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" s="11"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
+      <c r="C23" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s" s="8">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s" s="8">
+        <v>54</v>
+      </c>
+      <c r="F23" t="s" s="8">
+        <v>55</v>
+      </c>
+      <c r="G23" t="s" s="8">
+        <v>56</v>
+      </c>
       <c r="H23" s="10"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" s="11"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
+      <c r="C24" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s" s="8">
+        <v>90</v>
+      </c>
+      <c r="E24" t="s" s="8">
+        <v>91</v>
+      </c>
+      <c r="F24" t="s" s="8">
+        <v>92</v>
+      </c>
+      <c r="G24" t="s" s="8">
+        <v>93</v>
+      </c>
       <c r="H24" s="10"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" s="11"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
+      <c r="C25" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="E25" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="F25" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="G25" s="12">
+        <v>31172</v>
+      </c>
       <c r="H25" s="10"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" s="11"/>
       <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
+      <c r="C26" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="D26" t="s" s="8">
+        <v>94</v>
+      </c>
+      <c r="E26" t="s" s="8">
+        <v>95</v>
+      </c>
+      <c r="F26" t="s" s="8">
+        <v>96</v>
+      </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
+    </row>
+    <row r="27" ht="20.05" customHeight="1">
+      <c r="A27" s="11"/>
+      <c r="B27" s="9"/>
+      <c r="C27" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s" s="8">
+        <v>80</v>
+      </c>
+      <c r="E27" t="s" s="8">
+        <v>81</v>
+      </c>
+      <c r="F27" t="s" s="8">
+        <v>82</v>
+      </c>
+      <c r="G27" t="s" s="8">
+        <v>83</v>
+      </c>
+      <c r="H27" s="12">
+        <v>34734</v>
+      </c>
+    </row>
+    <row r="28" ht="20.05" customHeight="1">
+      <c r="A28" s="11"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+    </row>
+    <row r="29" ht="20.05" customHeight="1">
+      <c r="A29" s="11"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="10"/>
+      <c r="D29" t="s" s="8">
+        <v>97</v>
+      </c>
+      <c r="E29" t="s" s="8">
+        <v>98</v>
+      </c>
+      <c r="F29" t="s" s="8">
+        <v>99</v>
+      </c>
+      <c r="G29" t="s" s="8">
+        <v>100</v>
+      </c>
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" ht="20.05" customHeight="1">
+      <c r="A30" s="11"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" ht="20.05" customHeight="1">
+      <c r="A31" s="11"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" ht="20.05" customHeight="1">
+      <c r="A32" s="11"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2069,8 +2407,17 @@
     <hyperlink ref="D11" r:id="rId10" location="" tooltip="" display="rsykes1234@mail.com"/>
     <hyperlink ref="D12" r:id="rId11" location="" tooltip="" display="dkelly1234@mail.com"/>
     <hyperlink ref="D13" r:id="rId12" location="" tooltip="" display="rarnold1234@mail.com"/>
-    <hyperlink ref="D16" r:id="rId13" location="" tooltip="" display="twidel1234@mail.com"/>
-    <hyperlink ref="D17" r:id="rId14" location="" tooltip="" display="dkelly1234@mail.com"/>
+    <hyperlink ref="D14" r:id="rId13" location="" tooltip="" display="mwalters1234@mail.com"/>
+    <hyperlink ref="D15" r:id="rId14" location="" tooltip="" display="TestSanboxx12@outlook.com"/>
+    <hyperlink ref="D16" r:id="rId15" location="" tooltip="" display="lukehatfield721@gmail.com"/>
+    <hyperlink ref="D17" r:id="rId16" location="" tooltip="" display="rossvance247@gmail.com"/>
+    <hyperlink ref="D18" r:id="rId17" location="" tooltip="" display="rossvance247@gmail.com"/>
+    <hyperlink ref="D22" r:id="rId18" location="" tooltip="" display="twidel1234@mail.com"/>
+    <hyperlink ref="D23" r:id="rId19" location="" tooltip="" display="dkelly1234@mail.com"/>
+    <hyperlink ref="D24" r:id="rId20" location="" tooltip="" display="jkim1234@mail.com"/>
+    <hyperlink ref="D25" r:id="rId21" location="" tooltip="" display="lukehatfield721@gmail.com"/>
+    <hyperlink ref="D26" r:id="rId22" location="" tooltip="" display="rstone820@yahoo.com"/>
+    <hyperlink ref="D27" r:id="rId23" location="" tooltip="" display="rossvance247@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Added google registration, referral link, gift card tests
</commit_message>
<xml_diff>
--- a/src/main/java/com/sandboxx/dataManagement/testData/test_data.xlsx
+++ b/src/main/java/com/sandboxx/dataManagement/testData/test_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="122">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -130,6 +130,44 @@
     <t>Temp1234</t>
   </si>
   <si>
+    <t>jdoe12345@mail.com</t>
+  </si>
+  <si>
+    <t>4057704109</t>
+  </si>
+  <si>
+    <t>loginWithPhoneFail</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>rsykes1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Remi</t>
+  </si>
+  <si>
+    <t>Sykes</t>
+  </si>
+  <si>
+    <t>4328940918</t>
+  </si>
+  <si>
+    <t>logOutSuccess</t>
+  </si>
+  <si>
+    <t>registerWithEmail_ExistingEmail</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <u val="single"/>
@@ -141,41 +179,6 @@
     </r>
   </si>
   <si>
-    <t>4057704109</t>
-  </si>
-  <si>
-    <t>loginWithPhoneFail</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="14"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>rsykes1234@mail.com</t>
-    </r>
-  </si>
-  <si>
-    <t>Remi</t>
-  </si>
-  <si>
-    <t>Sykes</t>
-  </si>
-  <si>
-    <t>4328940918</t>
-  </si>
-  <si>
-    <t>logOutSuccess</t>
-  </si>
-  <si>
-    <t>registerWithEmail_ExistingEmail</t>
-  </si>
-  <si>
     <t>registerWithEmail_PhoneInUse</t>
   </si>
   <si>
@@ -373,6 +376,90 @@
   </si>
   <si>
     <t>registerWithGoogle_SendLetter</t>
+  </si>
+  <si>
+    <t>registerWithGoogle_DelayedEntryProgram</t>
+  </si>
+  <si>
+    <t>registerWithGoogle_DelayedEntryProgram_Trainee_Navy_GL</t>
+  </si>
+  <si>
+    <t>registerWithGoogle_ForceQuitAtBranchOfService</t>
+  </si>
+  <si>
+    <t>registerWithGoogle_Trainee_Marine_MA_GiftCards</t>
+  </si>
+  <si>
+    <t>registerWithGoogle_Trainee_Marine_MA_BuyGiftCard</t>
+  </si>
+  <si>
+    <t>generateReferralLink_noKin</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>acarrol1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Alivia</t>
+  </si>
+  <si>
+    <t>Carrol</t>
+  </si>
+  <si>
+    <t>2317633334</t>
+  </si>
+  <si>
+    <t>registerWithGoogle_FamilyAccount_AddRecipient</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>zarawalton254@gmail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Zara</t>
+  </si>
+  <si>
+    <t>Walton</t>
+  </si>
+  <si>
+    <t>7128800698</t>
+  </si>
+  <si>
+    <t>5/20/1989</t>
+  </si>
+  <si>
+    <t>generateReferralLink_WithKin</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>amata1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>Mata</t>
   </si>
   <si>
     <r>
@@ -1756,13 +1843,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="47.6875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="53.1719" style="1" customWidth="1"/>
     <col min="2" max="3" width="16.3516" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.8438" style="1" customWidth="1"/>
     <col min="5" max="8" width="16.3516" style="1" customWidth="1"/>
@@ -1944,7 +2031,7 @@
         <v>30</v>
       </c>
       <c r="D8" t="s" s="8">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s" s="8">
         <v>12</v>
@@ -1959,7 +2046,7 @@
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="6">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s" s="7">
         <v>34</v>
@@ -1968,44 +2055,44 @@
         <v>30</v>
       </c>
       <c r="D9" t="s" s="8">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s" s="8">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s" s="8">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G9" t="s" s="8">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="6">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" t="s" s="8">
         <v>30</v>
       </c>
       <c r="D10" t="s" s="8">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s" s="8">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F10" t="s" s="8">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G10" t="s" s="8">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="6">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" t="s" s="8">
@@ -2027,51 +2114,51 @@
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="6">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" t="s" s="8">
         <v>30</v>
       </c>
       <c r="D12" t="s" s="8">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s" s="8">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F12" t="s" s="8">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s" s="8">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H12" s="10"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="6">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" t="s" s="8">
         <v>30</v>
       </c>
       <c r="D13" t="s" s="8">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s" s="8">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s" s="8">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G13" t="s" s="8">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H13" s="10"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="6">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s" s="7">
         <v>34</v>
@@ -2080,235 +2167,289 @@
         <v>30</v>
       </c>
       <c r="D14" t="s" s="8">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s" s="8">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F14" t="s" s="8">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G14" t="s" s="8">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H14" s="10"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" t="s" s="6">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" t="s" s="8">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s" s="8">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s" s="8">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s" s="8">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G15" t="s" s="8">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H15" s="10"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="6">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" t="s" s="8">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s" s="8">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s" s="8">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s" s="8">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G16" t="s" s="8">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H16" t="s" s="8">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="6">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" t="s" s="8">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s" s="8">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s" s="8">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F17" t="s" s="8">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G17" t="s" s="8">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H17" t="s" s="8">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="6">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" t="s" s="8">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s" s="8">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s" s="8">
+        <v>82</v>
+      </c>
+      <c r="F18" t="s" s="8">
+        <v>83</v>
+      </c>
+      <c r="G18" t="s" s="8">
+        <v>84</v>
+      </c>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" ht="20.05" customHeight="1">
+      <c r="A19" t="s" s="6">
+        <v>87</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" t="s" s="8">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s" s="8">
         <v>81</v>
       </c>
-      <c r="F18" t="s" s="8">
+      <c r="E19" t="s" s="8">
         <v>82</v>
       </c>
-      <c r="G18" t="s" s="8">
+      <c r="F19" t="s" s="8">
         <v>83</v>
       </c>
-      <c r="H18" s="10"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
+      <c r="G19" t="s" s="8">
+        <v>84</v>
+      </c>
       <c r="H19" s="10"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="11"/>
+      <c r="A20" t="s" s="6">
+        <v>88</v>
+      </c>
       <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
+      <c r="C20" t="s" s="8">
+        <v>69</v>
+      </c>
+      <c r="D20" t="s" s="8">
+        <v>81</v>
+      </c>
+      <c r="E20" t="s" s="8">
+        <v>82</v>
+      </c>
+      <c r="F20" t="s" s="8">
+        <v>83</v>
+      </c>
+      <c r="G20" t="s" s="8">
+        <v>84</v>
+      </c>
       <c r="H20" s="10"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="11"/>
+      <c r="A21" t="s" s="6">
+        <v>89</v>
+      </c>
       <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="C21" t="s" s="8">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="F21" t="s" s="8">
+        <v>77</v>
+      </c>
+      <c r="G21" t="s" s="8">
+        <v>78</v>
+      </c>
+      <c r="H21" t="s" s="8">
+        <v>79</v>
+      </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="11"/>
+      <c r="A22" t="s" s="6">
+        <v>90</v>
+      </c>
       <c r="B22" s="9"/>
       <c r="C22" t="s" s="8">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s" s="8">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E22" t="s" s="8">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F22" t="s" s="8">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="G22" t="s" s="8">
-        <v>89</v>
-      </c>
-      <c r="H22" s="10"/>
+        <v>78</v>
+      </c>
+      <c r="H22" t="s" s="8">
+        <v>79</v>
+      </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="11"/>
+      <c r="A23" t="s" s="6">
+        <v>91</v>
+      </c>
       <c r="B23" s="9"/>
       <c r="C23" t="s" s="8">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s" s="8">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="E23" t="s" s="8">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="F23" t="s" s="8">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="G23" t="s" s="8">
-        <v>56</v>
-      </c>
-      <c r="H23" s="10"/>
+        <v>78</v>
+      </c>
+      <c r="H23" t="s" s="8">
+        <v>79</v>
+      </c>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="11"/>
+      <c r="A24" t="s" s="6">
+        <v>92</v>
+      </c>
       <c r="B24" s="9"/>
       <c r="C24" t="s" s="8">
         <v>30</v>
       </c>
       <c r="D24" t="s" s="8">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E24" t="s" s="8">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F24" t="s" s="8">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G24" t="s" s="8">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H24" s="10"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="11"/>
+      <c r="A25" t="s" s="6">
+        <v>97</v>
+      </c>
       <c r="B25" s="9"/>
       <c r="C25" t="s" s="8">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D25" t="s" s="8">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="E25" t="s" s="8">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="F25" t="s" s="8">
-        <v>76</v>
-      </c>
-      <c r="G25" s="12">
-        <v>31172</v>
-      </c>
-      <c r="H25" s="10"/>
+        <v>100</v>
+      </c>
+      <c r="G25" t="s" s="8">
+        <v>101</v>
+      </c>
+      <c r="H25" t="s" s="8">
+        <v>102</v>
+      </c>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="11"/>
+      <c r="A26" t="s" s="6">
+        <v>103</v>
+      </c>
       <c r="B26" s="9"/>
       <c r="C26" t="s" s="8">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s" s="8">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E26" t="s" s="8">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="F26" t="s" s="8">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
@@ -2316,24 +2457,12 @@
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" s="11"/>
       <c r="B27" s="9"/>
-      <c r="C27" t="s" s="8">
-        <v>68</v>
-      </c>
-      <c r="D27" t="s" s="8">
-        <v>80</v>
-      </c>
-      <c r="E27" t="s" s="8">
-        <v>81</v>
-      </c>
-      <c r="F27" t="s" s="8">
-        <v>82</v>
-      </c>
-      <c r="G27" t="s" s="8">
-        <v>83</v>
-      </c>
-      <c r="H27" s="12">
-        <v>34734</v>
-      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" s="11"/>
@@ -2349,18 +2478,10 @@
       <c r="A29" s="11"/>
       <c r="B29" s="9"/>
       <c r="C29" s="10"/>
-      <c r="D29" t="s" s="8">
-        <v>97</v>
-      </c>
-      <c r="E29" t="s" s="8">
-        <v>98</v>
-      </c>
-      <c r="F29" t="s" s="8">
-        <v>99</v>
-      </c>
-      <c r="G29" t="s" s="8">
-        <v>100</v>
-      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
       <c r="H29" s="10"/>
     </row>
     <row r="30" ht="20.05" customHeight="1">
@@ -2386,38 +2507,213 @@
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" s="11"/>
       <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
+      <c r="C32" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s" s="8">
+        <v>107</v>
+      </c>
+      <c r="E32" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="F32" t="s" s="8">
+        <v>109</v>
+      </c>
+      <c r="G32" t="s" s="8">
+        <v>110</v>
+      </c>
       <c r="H32" s="10"/>
+    </row>
+    <row r="33" ht="20.05" customHeight="1">
+      <c r="A33" s="11"/>
+      <c r="B33" s="9"/>
+      <c r="C33" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s" s="8">
+        <v>54</v>
+      </c>
+      <c r="E33" t="s" s="8">
+        <v>55</v>
+      </c>
+      <c r="F33" t="s" s="8">
+        <v>56</v>
+      </c>
+      <c r="G33" t="s" s="8">
+        <v>57</v>
+      </c>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" ht="20.05" customHeight="1">
+      <c r="A34" s="11"/>
+      <c r="B34" s="9"/>
+      <c r="C34" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="D34" t="s" s="8">
+        <v>111</v>
+      </c>
+      <c r="E34" t="s" s="8">
+        <v>112</v>
+      </c>
+      <c r="F34" t="s" s="8">
+        <v>113</v>
+      </c>
+      <c r="G34" t="s" s="8">
+        <v>114</v>
+      </c>
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" ht="20.05" customHeight="1">
+      <c r="A35" s="11"/>
+      <c r="B35" s="9"/>
+      <c r="C35" t="s" s="8">
+        <v>69</v>
+      </c>
+      <c r="D35" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="E35" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="F35" t="s" s="8">
+        <v>77</v>
+      </c>
+      <c r="G35" s="12">
+        <v>31172</v>
+      </c>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" ht="20.05" customHeight="1">
+      <c r="A36" s="11"/>
+      <c r="B36" s="9"/>
+      <c r="C36" t="s" s="8">
+        <v>69</v>
+      </c>
+      <c r="D36" t="s" s="8">
+        <v>115</v>
+      </c>
+      <c r="E36" t="s" s="8">
+        <v>116</v>
+      </c>
+      <c r="F36" t="s" s="8">
+        <v>117</v>
+      </c>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+    </row>
+    <row r="37" ht="20.05" customHeight="1">
+      <c r="A37" s="11"/>
+      <c r="B37" s="9"/>
+      <c r="C37" t="s" s="8">
+        <v>69</v>
+      </c>
+      <c r="D37" t="s" s="8">
+        <v>81</v>
+      </c>
+      <c r="E37" t="s" s="8">
+        <v>82</v>
+      </c>
+      <c r="F37" t="s" s="8">
+        <v>83</v>
+      </c>
+      <c r="G37" t="s" s="8">
+        <v>84</v>
+      </c>
+      <c r="H37" s="12">
+        <v>34734</v>
+      </c>
+    </row>
+    <row r="38" ht="20.05" customHeight="1">
+      <c r="A38" s="11"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+    </row>
+    <row r="39" ht="20.05" customHeight="1">
+      <c r="A39" s="11"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="10"/>
+      <c r="D39" t="s" s="8">
+        <v>118</v>
+      </c>
+      <c r="E39" t="s" s="8">
+        <v>119</v>
+      </c>
+      <c r="F39" t="s" s="8">
+        <v>120</v>
+      </c>
+      <c r="G39" t="s" s="8">
+        <v>121</v>
+      </c>
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" ht="20.05" customHeight="1">
+      <c r="A40" s="11"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+    </row>
+    <row r="41" ht="20.05" customHeight="1">
+      <c r="A41" s="11"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" ht="20.05" customHeight="1">
+      <c r="A42" s="11"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" location="" tooltip="" display="myemail@mail.com"/>
     <hyperlink ref="D3" r:id="rId2" location="" tooltip="" display="myemail2@mail.com"/>
     <hyperlink ref="D4" r:id="rId3" location="" tooltip="" display="myemail3@mail.com"/>
-    <hyperlink ref="D5" r:id="rId4" location="" tooltip="" display="jdoe1234@mail.com"/>
-    <hyperlink ref="D6" r:id="rId5" location="" tooltip="" display="rsykes1234@mail.com"/>
-    <hyperlink ref="D7" r:id="rId6" location="" tooltip="" display="rsykes1234@mail.com"/>
-    <hyperlink ref="D8" r:id="rId7" location="" tooltip="" display="jdoe1234@mail.com"/>
-    <hyperlink ref="D9" r:id="rId8" location="" tooltip="" display="ihunter1234@mail.com"/>
-    <hyperlink ref="D10" r:id="rId9" location="" tooltip="" display="cgonzales1234@mail.com"/>
-    <hyperlink ref="D11" r:id="rId10" location="" tooltip="" display="rsykes1234@mail.com"/>
-    <hyperlink ref="D12" r:id="rId11" location="" tooltip="" display="dkelly1234@mail.com"/>
-    <hyperlink ref="D13" r:id="rId12" location="" tooltip="" display="rarnold1234@mail.com"/>
-    <hyperlink ref="D14" r:id="rId13" location="" tooltip="" display="mwalters1234@mail.com"/>
-    <hyperlink ref="D15" r:id="rId14" location="" tooltip="" display="TestSanboxx12@outlook.com"/>
-    <hyperlink ref="D16" r:id="rId15" location="" tooltip="" display="lukehatfield721@gmail.com"/>
-    <hyperlink ref="D17" r:id="rId16" location="" tooltip="" display="rossvance247@gmail.com"/>
-    <hyperlink ref="D18" r:id="rId17" location="" tooltip="" display="rossvance247@gmail.com"/>
-    <hyperlink ref="D22" r:id="rId18" location="" tooltip="" display="twidel1234@mail.com"/>
-    <hyperlink ref="D23" r:id="rId19" location="" tooltip="" display="dkelly1234@mail.com"/>
-    <hyperlink ref="D24" r:id="rId20" location="" tooltip="" display="jkim1234@mail.com"/>
-    <hyperlink ref="D25" r:id="rId21" location="" tooltip="" display="lukehatfield721@gmail.com"/>
-    <hyperlink ref="D26" r:id="rId22" location="" tooltip="" display="rstone820@yahoo.com"/>
-    <hyperlink ref="D27" r:id="rId23" location="" tooltip="" display="rossvance247@gmail.com"/>
+    <hyperlink ref="D6" r:id="rId4" location="" tooltip="" display="rsykes1234@mail.com"/>
+    <hyperlink ref="D7" r:id="rId5" location="" tooltip="" display="rsykes1234@mail.com"/>
+    <hyperlink ref="D8" r:id="rId6" location="" tooltip="" display="jdoe1234@mail.com"/>
+    <hyperlink ref="D9" r:id="rId7" location="" tooltip="" display="ihunter1234@mail.com"/>
+    <hyperlink ref="D10" r:id="rId8" location="" tooltip="" display="cgonzales1234@mail.com"/>
+    <hyperlink ref="D11" r:id="rId9" location="" tooltip="" display="rsykes1234@mail.com"/>
+    <hyperlink ref="D12" r:id="rId10" location="" tooltip="" display="dkelly1234@mail.com"/>
+    <hyperlink ref="D13" r:id="rId11" location="" tooltip="" display="rarnold1234@mail.com"/>
+    <hyperlink ref="D14" r:id="rId12" location="" tooltip="" display="mwalters1234@mail.com"/>
+    <hyperlink ref="D15" r:id="rId13" location="" tooltip="" display="TestSanboxx12@outlook.com"/>
+    <hyperlink ref="D16" r:id="rId14" location="" tooltip="" display="lukehatfield721@gmail.com"/>
+    <hyperlink ref="D17" r:id="rId15" location="" tooltip="" display="rossvance247@gmail.com"/>
+    <hyperlink ref="D18" r:id="rId16" location="" tooltip="" display="rossvance247@gmail.com"/>
+    <hyperlink ref="D19" r:id="rId17" location="" tooltip="" display="rossvance247@gmail.com"/>
+    <hyperlink ref="D20" r:id="rId18" location="" tooltip="" display="rossvance247@gmail.com"/>
+    <hyperlink ref="D21" r:id="rId19" location="" tooltip="" display="lukehatfield721@gmail.com"/>
+    <hyperlink ref="D22" r:id="rId20" location="" tooltip="" display="lukehatfield721@gmail.com"/>
+    <hyperlink ref="D23" r:id="rId21" location="" tooltip="" display="lukehatfield721@gmail.com"/>
+    <hyperlink ref="D24" r:id="rId22" location="" tooltip="" display="acarrol1234@mail.com"/>
+    <hyperlink ref="D25" r:id="rId23" location="" tooltip="" display="zarawalton254@gmail.com"/>
+    <hyperlink ref="D26" r:id="rId24" location="" tooltip="" display="amata1234@mail.com"/>
+    <hyperlink ref="D32" r:id="rId25" location="" tooltip="" display="twidel1234@mail.com"/>
+    <hyperlink ref="D33" r:id="rId26" location="" tooltip="" display="dkelly1234@mail.com"/>
+    <hyperlink ref="D34" r:id="rId27" location="" tooltip="" display="jkim1234@mail.com"/>
+    <hyperlink ref="D35" r:id="rId28" location="" tooltip="" display="lukehatfield721@gmail.com"/>
+    <hyperlink ref="D36" r:id="rId29" location="" tooltip="" display="rstone820@yahoo.com"/>
+    <hyperlink ref="D37" r:id="rId30" location="" tooltip="" display="rossvance247@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Added Address Book tests
</commit_message>
<xml_diff>
--- a/src/main/java/com/sandboxx/dataManagement/testData/test_data.xlsx
+++ b/src/main/java/com/sandboxx/dataManagement/testData/test_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="160">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -66,64 +66,6 @@
     <t>7732548005</t>
   </si>
   <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Username2</t>
-  </si>
-  <si>
-    <t>Password2</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="14"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>myemail2@mail.com</t>
-    </r>
-  </si>
-  <si>
-    <t>Mike</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>2025460025</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>Username3</t>
-  </si>
-  <si>
-    <t>Password3</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="14"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>myemail3@mail.com</t>
-    </r>
-  </si>
-  <si>
-    <t>Kathy</t>
-  </si>
-  <si>
-    <t>Jonson</t>
-  </si>
-  <si>
-    <t>3452352344</t>
-  </si>
-  <si>
     <t>registerWithEmail_AutoConnectedKin</t>
   </si>
   <si>
@@ -165,18 +107,26 @@
     <t>logOutSuccess</t>
   </si>
   <si>
-    <t>registerWithEmail_ExistingEmail</t>
-  </si>
-  <si>
     <r>
       <rPr>
-        <u val="single"/>
         <sz val="10"/>
-        <color indexed="14"/>
+        <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>jdoe1234@mail.com</t>
+      <t>rsykes1234@mail.com</t>
     </r>
+  </si>
+  <si>
+    <t>registerWithEmail_ExistingEmail</t>
+  </si>
+  <si>
+    <t>bcastillo1234@mail.com</t>
+  </si>
+  <si>
+    <t>Betsy</t>
+  </si>
+  <si>
+    <t>Castillo</t>
   </si>
   <si>
     <t>registerWithEmail_PhoneInUse</t>
@@ -207,9 +157,8 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
         <sz val="10"/>
-        <color indexed="14"/>
+        <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>cgonzales1234@mail.com</t>
@@ -460,6 +409,177 @@
   </si>
   <si>
     <t>Mata</t>
+  </si>
+  <si>
+    <t>registerJoiningMilitaryAccountWithEmail</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>psims1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Sims</t>
+  </si>
+  <si>
+    <t>3348361884</t>
+  </si>
+  <si>
+    <t>registerNewRecruiter</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>lbyrne1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Lillie</t>
+  </si>
+  <si>
+    <t>Byrne</t>
+  </si>
+  <si>
+    <t>4704493228</t>
+  </si>
+  <si>
+    <t>RecruitFirst:Brian,RecruitLast:Carter,RecruitEmail:bcarter1234@mail.com</t>
+  </si>
+  <si>
+    <t>registerNewRecruitWithEmail_ConnectRecruiter</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>bcarter1234@mail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>recruiterVerifyConnectedRecruit</t>
+  </si>
+  <si>
+    <t>Address Book Via Letter Compose Tests</t>
+  </si>
+  <si>
+    <t>purchaseBundle_20Letters</t>
+  </si>
+  <si>
+    <t>kmcintyre1234@mail.com</t>
+  </si>
+  <si>
+    <t>Keaton</t>
+  </si>
+  <si>
+    <t>Mcintyre</t>
+  </si>
+  <si>
+    <t>sendLetterWithNewContact</t>
+  </si>
+  <si>
+    <t>Address1:1234 Kedzie st,City:Dundee,State:WV,Zip:50068</t>
+  </si>
+  <si>
+    <t>sendLetterWithNewContact_AddressFormatter</t>
+  </si>
+  <si>
+    <t>sendLetterWithEditedContact</t>
+  </si>
+  <si>
+    <t>sendLetter_DeleteContact</t>
+  </si>
+  <si>
+    <t>addAutoconnectedContact_SendLetter_ValidAddress</t>
+  </si>
+  <si>
+    <t>6702069893693440</t>
+  </si>
+  <si>
+    <t>ContactFirst:Conrad,ContactLast:Hobbs,ContactEmail:chobbs1234@mail.com,ContactPassword:Temp1234,Address:346 Colfax st,City:Oakville,State:CO,Zip:10125</t>
+  </si>
+  <si>
+    <t>sendLetterToConnection_Fail_InvalidAddress</t>
+  </si>
+  <si>
+    <t>6683982410678272</t>
+  </si>
+  <si>
+    <t>ContactFirst:Lea,ContactLast:Rivera,ContactEmail:lrivera1234@mail.com,ContactPassword:Temp1234,Address:346 Colfax st,City:Oakville,State:CO,Zip:10125</t>
+  </si>
+  <si>
+    <t>sendLetterToNotConnectedRecipient</t>
+  </si>
+  <si>
+    <t>rgentry1234@mail.com</t>
+  </si>
+  <si>
+    <t>Ruairi</t>
+  </si>
+  <si>
+    <t>Gentry</t>
+  </si>
+  <si>
+    <t>ContactFirst:Hallie,ContactLast:Thomas,ContactEmail:hthomas1234@mail.com,ContactPassword:Temp1234,Address:650 Stark st,City:Caster,State:IL,Zip:50020</t>
+  </si>
+  <si>
+    <t>Address Book Test</t>
+  </si>
+  <si>
+    <t>createNewContactWithManualAddressEntry_ToChangeTest</t>
+  </si>
+  <si>
+    <t>sbartlet1234@mail.com</t>
+  </si>
+  <si>
+    <t>Samson</t>
+  </si>
+  <si>
+    <t>Bartlet</t>
+  </si>
+  <si>
+    <t>addressBook_ViewContactsAndConnections</t>
+  </si>
+  <si>
+    <t>lsimmons1234@mail.com</t>
+  </si>
+  <si>
+    <t>Leroy</t>
+  </si>
+  <si>
+    <t>Simmons</t>
+  </si>
+  <si>
+    <t>createNewContactWithManualAddressEntry</t>
+  </si>
+  <si>
+    <t>createNewContactWithAddressFormatter</t>
+  </si>
+  <si>
+    <t>ContactFirst:Helena,ContactLast:Barr,RankType:MARINES,Rank:RCT,Base:GREAT LAKES,Ship:ship5,Division:123</t>
   </si>
   <si>
     <r>
@@ -741,16 +861,16 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1843,16 +1963,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="53.1719" style="1" customWidth="1"/>
-    <col min="2" max="3" width="16.3516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.8438" style="1" customWidth="1"/>
-    <col min="5" max="8" width="16.3516" style="1" customWidth="1"/>
+    <col min="5" max="7" width="16.3516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="63" style="1" customWidth="1"/>
     <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1910,237 +2032,235 @@
       <c r="A3" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="B3" s="7"/>
+      <c r="C3" t="s" s="8">
         <v>16</v>
       </c>
-      <c r="C3" t="s" s="8">
+      <c r="D3" t="s" s="8">
         <v>17</v>
       </c>
-      <c r="D3" t="s" s="8">
+      <c r="E3" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s" s="8">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="E3" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s" s="8">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="H3" s="8"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s" s="8">
         <v>22</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="F4" t="s" s="8">
         <v>23</v>
       </c>
-      <c r="C4" t="s" s="8">
+      <c r="G4" t="s" s="8">
         <v>24</v>
       </c>
-      <c r="D4" t="s" s="8">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s" s="8">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s" s="8">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s" s="8">
-        <v>28</v>
-      </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" t="s" s="6">
-        <v>29</v>
-      </c>
-      <c r="B5" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="B5" s="7"/>
       <c r="C5" t="s" s="8">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s" s="8">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s" s="8">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s" s="8">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s" s="8">
-        <v>32</v>
-      </c>
-      <c r="H5" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="6">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s" s="7">
-        <v>34</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B6" s="7"/>
       <c r="C6" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s" s="8">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s" s="8">
         <v>30</v>
       </c>
-      <c r="D6" t="s" s="8">
-        <v>35</v>
-      </c>
-      <c r="E6" t="s" s="8">
-        <v>36</v>
-      </c>
-      <c r="F6" t="s" s="8">
-        <v>37</v>
-      </c>
       <c r="G6" t="s" s="8">
-        <v>38</v>
-      </c>
-      <c r="H6" s="10"/>
+        <v>18</v>
+      </c>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="6">
-        <v>39</v>
-      </c>
-      <c r="B7" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="B7" t="s" s="10">
+        <v>20</v>
+      </c>
       <c r="C7" t="s" s="8">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s" s="8">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s" s="8">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s" s="8">
         <v>35</v>
       </c>
-      <c r="E7" t="s" s="8">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s" s="8">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s" s="8">
-        <v>38</v>
-      </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="6">
+        <v>36</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s" s="8">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s" s="8">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s" s="8">
+        <v>39</v>
+      </c>
+      <c r="G8" t="s" s="8">
         <v>40</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" t="s" s="8">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s" s="8">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s" s="8">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s" s="8">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s" s="8">
-        <v>32</v>
-      </c>
-      <c r="H8" s="10"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="6">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s" s="7">
-        <v>34</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="B9" s="7"/>
       <c r="C9" t="s" s="8">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s" s="8">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s" s="8">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s" s="8">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s" s="8">
-        <v>46</v>
-      </c>
-      <c r="H9" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="6">
-        <v>47</v>
-      </c>
-      <c r="B10" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="B10" s="7"/>
       <c r="C10" t="s" s="8">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s" s="8">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s" s="8">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s" s="8">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G10" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="H10" s="10"/>
+        <v>46</v>
+      </c>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="6">
-        <v>52</v>
-      </c>
-      <c r="B11" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="B11" s="7"/>
       <c r="C11" t="s" s="8">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s" s="8">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s" s="8">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s" s="8">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s" s="8">
-        <v>38</v>
-      </c>
-      <c r="H11" s="10"/>
+        <v>51</v>
+      </c>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="6">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s" s="8">
         <v>53</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" t="s" s="8">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s" s="8">
+      <c r="E12" t="s" s="8">
         <v>54</v>
       </c>
-      <c r="E12" t="s" s="8">
+      <c r="F12" t="s" s="8">
         <v>55</v>
       </c>
-      <c r="F12" t="s" s="8">
+      <c r="G12" t="s" s="8">
         <v>56</v>
       </c>
-      <c r="G12" t="s" s="8">
-        <v>57</v>
-      </c>
-      <c r="H12" s="10"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="6">
+        <v>57</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" t="s" s="8">
         <v>58</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" t="s" s="8">
-        <v>30</v>
       </c>
       <c r="D13" t="s" s="8">
         <v>59</v>
@@ -2154,17 +2274,15 @@
       <c r="G13" t="s" s="8">
         <v>62</v>
       </c>
-      <c r="H13" s="10"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="6">
         <v>63</v>
       </c>
-      <c r="B14" t="s" s="7">
-        <v>34</v>
-      </c>
+      <c r="B14" s="7"/>
       <c r="C14" t="s" s="8">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s" s="8">
         <v>64</v>
@@ -2178,15 +2296,17 @@
       <c r="G14" t="s" s="8">
         <v>67</v>
       </c>
-      <c r="H14" s="10"/>
+      <c r="H14" t="s" s="8">
+        <v>68</v>
+      </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" t="s" s="6">
-        <v>68</v>
-      </c>
-      <c r="B15" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="B15" s="7"/>
       <c r="C15" t="s" s="8">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s" s="8">
         <v>70</v>
@@ -2200,201 +2320,201 @@
       <c r="G15" t="s" s="8">
         <v>73</v>
       </c>
-      <c r="H15" s="10"/>
+      <c r="H15" t="s" s="8">
+        <v>74</v>
+      </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="6">
-        <v>74</v>
-      </c>
-      <c r="B16" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="B16" s="7"/>
       <c r="C16" t="s" s="8">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s" s="8">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s" s="8">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F16" t="s" s="8">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G16" t="s" s="8">
-        <v>78</v>
-      </c>
-      <c r="H16" t="s" s="8">
-        <v>79</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="6">
-        <v>80</v>
-      </c>
-      <c r="B17" s="9"/>
+        <v>76</v>
+      </c>
+      <c r="B17" s="7"/>
       <c r="C17" t="s" s="8">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s" s="8">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s" s="8">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="F17" t="s" s="8">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G17" t="s" s="8">
-        <v>84</v>
-      </c>
-      <c r="H17" t="s" s="8">
-        <v>85</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="6">
-        <v>86</v>
-      </c>
-      <c r="B18" s="9"/>
+        <v>77</v>
+      </c>
+      <c r="B18" s="7"/>
       <c r="C18" t="s" s="8">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s" s="8">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="E18" t="s" s="8">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="F18" t="s" s="8">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G18" t="s" s="8">
-        <v>84</v>
-      </c>
-      <c r="H18" s="10"/>
+        <v>73</v>
+      </c>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="6">
-        <v>87</v>
-      </c>
-      <c r="B19" s="9"/>
+        <v>78</v>
+      </c>
+      <c r="B19" s="7"/>
       <c r="C19" t="s" s="8">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s" s="8">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s" s="8">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s" s="8">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="G19" t="s" s="8">
-        <v>84</v>
-      </c>
-      <c r="H19" s="10"/>
+        <v>67</v>
+      </c>
+      <c r="H19" t="s" s="8">
+        <v>68</v>
+      </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="6">
-        <v>88</v>
-      </c>
-      <c r="B20" s="9"/>
+        <v>79</v>
+      </c>
+      <c r="B20" s="7"/>
       <c r="C20" t="s" s="8">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s" s="8">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s" s="8">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F20" t="s" s="8">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="G20" t="s" s="8">
-        <v>84</v>
-      </c>
-      <c r="H20" s="10"/>
+        <v>67</v>
+      </c>
+      <c r="H20" t="s" s="8">
+        <v>68</v>
+      </c>
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="6">
-        <v>89</v>
-      </c>
-      <c r="B21" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="B21" s="7"/>
       <c r="C21" t="s" s="8">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s" s="8">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s" s="8">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="F21" t="s" s="8">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G21" t="s" s="8">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="H21" t="s" s="8">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="6">
-        <v>90</v>
-      </c>
-      <c r="B22" s="9"/>
+        <v>81</v>
+      </c>
+      <c r="B22" s="7"/>
       <c r="C22" t="s" s="8">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s" s="8">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E22" t="s" s="8">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="F22" t="s" s="8">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="G22" t="s" s="8">
-        <v>78</v>
-      </c>
-      <c r="H22" t="s" s="8">
-        <v>79</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="6">
+        <v>86</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" t="s" s="8">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s" s="8">
+        <v>87</v>
+      </c>
+      <c r="E23" t="s" s="8">
+        <v>88</v>
+      </c>
+      <c r="F23" t="s" s="8">
+        <v>89</v>
+      </c>
+      <c r="G23" t="s" s="8">
+        <v>90</v>
+      </c>
+      <c r="H23" t="s" s="8">
         <v>91</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" t="s" s="8">
-        <v>69</v>
-      </c>
-      <c r="D23" t="s" s="8">
-        <v>75</v>
-      </c>
-      <c r="E23" t="s" s="8">
-        <v>76</v>
-      </c>
-      <c r="F23" t="s" s="8">
-        <v>77</v>
-      </c>
-      <c r="G23" t="s" s="8">
-        <v>78</v>
-      </c>
-      <c r="H23" t="s" s="8">
-        <v>79</v>
       </c>
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="6">
         <v>92</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" s="7"/>
       <c r="C24" t="s" s="8">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s" s="8">
         <v>93</v>
@@ -2405,315 +2525,608 @@
       <c r="F24" t="s" s="8">
         <v>95</v>
       </c>
-      <c r="G24" t="s" s="8">
-        <v>96</v>
-      </c>
-      <c r="H24" s="10"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" t="s" s="6">
+        <v>96</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D25" t="s" s="8">
         <v>97</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" t="s" s="8">
-        <v>69</v>
-      </c>
-      <c r="D25" t="s" s="8">
+      <c r="E25" t="s" s="8">
         <v>98</v>
       </c>
-      <c r="E25" t="s" s="8">
+      <c r="F25" t="s" s="8">
         <v>99</v>
       </c>
-      <c r="F25" t="s" s="8">
+      <c r="G25" t="s" s="8">
         <v>100</v>
       </c>
-      <c r="G25" t="s" s="8">
-        <v>101</v>
-      </c>
-      <c r="H25" t="s" s="8">
-        <v>102</v>
-      </c>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="6">
+        <v>101</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s" s="8">
+        <v>102</v>
+      </c>
+      <c r="E26" t="s" s="8">
         <v>103</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" t="s" s="8">
-        <v>30</v>
-      </c>
-      <c r="D26" t="s" s="8">
+      <c r="F26" t="s" s="8">
         <v>104</v>
       </c>
-      <c r="E26" t="s" s="8">
+      <c r="G26" t="s" s="8">
         <v>105</v>
       </c>
-      <c r="F26" t="s" s="8">
+      <c r="H26" t="s" s="8">
         <v>106</v>
       </c>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
+      <c r="A27" t="s" s="6">
+        <v>107</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s" s="8">
+        <v>108</v>
+      </c>
+      <c r="E27" t="s" s="8">
+        <v>109</v>
+      </c>
+      <c r="F27" t="s" s="8">
+        <v>110</v>
+      </c>
+      <c r="G27" t="s" s="8">
+        <v>105</v>
+      </c>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
+      <c r="A28" t="s" s="6">
+        <v>111</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s" s="8">
+        <v>102</v>
+      </c>
+      <c r="E28" t="s" s="8">
+        <v>103</v>
+      </c>
+      <c r="F28" t="s" s="8">
+        <v>104</v>
+      </c>
+      <c r="G28" t="s" s="8">
+        <v>105</v>
+      </c>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
+      <c r="A29" t="s" s="6">
+        <v>112</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
+      <c r="A30" t="s" s="6">
+        <v>113</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D30" t="s" s="8">
+        <v>114</v>
+      </c>
+      <c r="E30" t="s" s="8">
+        <v>115</v>
+      </c>
+      <c r="F30" t="s" s="8">
+        <v>116</v>
+      </c>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" s="11"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
+      <c r="A31" t="s" s="6">
+        <v>117</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s" s="8">
+        <v>114</v>
+      </c>
+      <c r="E31" t="s" s="8">
+        <v>115</v>
+      </c>
+      <c r="F31" t="s" s="8">
+        <v>116</v>
+      </c>
+      <c r="G31" s="9"/>
+      <c r="H31" t="s" s="8">
+        <v>118</v>
+      </c>
     </row>
     <row r="32" ht="20.05" customHeight="1">
-      <c r="A32" s="11"/>
-      <c r="B32" s="9"/>
+      <c r="A32" t="s" s="6">
+        <v>119</v>
+      </c>
+      <c r="B32" s="7"/>
       <c r="C32" t="s" s="8">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D32" t="s" s="8">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="E32" t="s" s="8">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="F32" t="s" s="8">
-        <v>109</v>
-      </c>
-      <c r="G32" t="s" s="8">
-        <v>110</v>
-      </c>
-      <c r="H32" s="10"/>
+        <v>116</v>
+      </c>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" ht="20.05" customHeight="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="9"/>
+      <c r="A33" t="s" s="6">
+        <v>120</v>
+      </c>
+      <c r="B33" s="7"/>
       <c r="C33" t="s" s="8">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D33" t="s" s="8">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="E33" t="s" s="8">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="F33" t="s" s="8">
-        <v>56</v>
-      </c>
-      <c r="G33" t="s" s="8">
-        <v>57</v>
-      </c>
-      <c r="H33" s="10"/>
+        <v>116</v>
+      </c>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
     </row>
     <row r="34" ht="20.05" customHeight="1">
-      <c r="A34" s="11"/>
-      <c r="B34" s="9"/>
+      <c r="A34" t="s" s="6">
+        <v>121</v>
+      </c>
+      <c r="B34" s="7"/>
       <c r="C34" t="s" s="8">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D34" t="s" s="8">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E34" t="s" s="8">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F34" t="s" s="8">
-        <v>113</v>
-      </c>
-      <c r="G34" t="s" s="8">
+        <v>116</v>
+      </c>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+    </row>
+    <row r="35" ht="20.05" customHeight="1">
+      <c r="A35" t="s" s="6">
+        <v>122</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s" s="8">
         <v>114</v>
       </c>
-      <c r="H34" s="10"/>
-    </row>
-    <row r="35" ht="20.05" customHeight="1">
-      <c r="A35" s="11"/>
-      <c r="B35" s="9"/>
-      <c r="C35" t="s" s="8">
-        <v>69</v>
-      </c>
-      <c r="D35" t="s" s="8">
-        <v>75</v>
-      </c>
       <c r="E35" t="s" s="8">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="F35" t="s" s="8">
-        <v>77</v>
-      </c>
-      <c r="G35" s="12">
+        <v>116</v>
+      </c>
+      <c r="G35" t="s" s="8">
+        <v>123</v>
+      </c>
+      <c r="H35" t="s" s="8">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" ht="20.05" customHeight="1">
+      <c r="A36" t="s" s="6">
+        <v>125</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D36" t="s" s="8">
+        <v>114</v>
+      </c>
+      <c r="E36" t="s" s="8">
+        <v>115</v>
+      </c>
+      <c r="F36" t="s" s="8">
+        <v>116</v>
+      </c>
+      <c r="G36" t="s" s="8">
+        <v>126</v>
+      </c>
+      <c r="H36" t="s" s="8">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" ht="20.05" customHeight="1">
+      <c r="A37" t="s" s="6">
+        <v>128</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D37" t="s" s="8">
+        <v>129</v>
+      </c>
+      <c r="E37" t="s" s="8">
+        <v>130</v>
+      </c>
+      <c r="F37" t="s" s="8">
+        <v>131</v>
+      </c>
+      <c r="G37" s="9"/>
+      <c r="H37" t="s" s="8">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" ht="20.05" customHeight="1">
+      <c r="A38" t="s" s="6">
+        <v>133</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" ht="20.05" customHeight="1">
+      <c r="A39" t="s" s="6">
+        <v>134</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D39" t="s" s="8">
+        <v>135</v>
+      </c>
+      <c r="E39" t="s" s="8">
+        <v>136</v>
+      </c>
+      <c r="F39" t="s" s="8">
+        <v>137</v>
+      </c>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+    </row>
+    <row r="40" ht="20.05" customHeight="1">
+      <c r="A40" t="s" s="6">
+        <v>138</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D40" t="s" s="8">
+        <v>139</v>
+      </c>
+      <c r="E40" t="s" s="8">
+        <v>140</v>
+      </c>
+      <c r="F40" t="s" s="8">
+        <v>141</v>
+      </c>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" ht="20.05" customHeight="1">
+      <c r="A41" t="s" s="6">
+        <v>142</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D41" t="s" s="8">
+        <v>139</v>
+      </c>
+      <c r="E41" t="s" s="8">
+        <v>140</v>
+      </c>
+      <c r="F41" t="s" s="8">
+        <v>141</v>
+      </c>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" ht="20.05" customHeight="1">
+      <c r="A42" t="s" s="6">
+        <v>143</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D42" t="s" s="8">
+        <v>139</v>
+      </c>
+      <c r="E42" t="s" s="8">
+        <v>140</v>
+      </c>
+      <c r="F42" t="s" s="8">
+        <v>141</v>
+      </c>
+      <c r="G42" s="9"/>
+      <c r="H42" t="s" s="8">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" ht="20.05" customHeight="1">
+      <c r="A43" s="11"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+    </row>
+    <row r="44" ht="20.05" customHeight="1">
+      <c r="A44" s="11"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+    </row>
+    <row r="45" ht="20.05" customHeight="1">
+      <c r="A45" s="11"/>
+      <c r="B45" s="7"/>
+      <c r="C45" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D45" t="s" s="8">
+        <v>145</v>
+      </c>
+      <c r="E45" t="s" s="8">
+        <v>146</v>
+      </c>
+      <c r="F45" t="s" s="8">
+        <v>147</v>
+      </c>
+      <c r="G45" t="s" s="8">
+        <v>148</v>
+      </c>
+      <c r="H45" s="9"/>
+    </row>
+    <row r="46" ht="20.05" customHeight="1">
+      <c r="A46" s="11"/>
+      <c r="B46" s="7"/>
+      <c r="C46" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D46" t="s" s="8">
+        <v>43</v>
+      </c>
+      <c r="E46" t="s" s="8">
+        <v>44</v>
+      </c>
+      <c r="F46" t="s" s="8">
+        <v>45</v>
+      </c>
+      <c r="G46" t="s" s="8">
+        <v>46</v>
+      </c>
+      <c r="H46" s="9"/>
+    </row>
+    <row r="47" ht="20.05" customHeight="1">
+      <c r="A47" s="11"/>
+      <c r="B47" s="7"/>
+      <c r="C47" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="D47" t="s" s="8">
+        <v>149</v>
+      </c>
+      <c r="E47" t="s" s="8">
+        <v>150</v>
+      </c>
+      <c r="F47" t="s" s="8">
+        <v>151</v>
+      </c>
+      <c r="G47" t="s" s="8">
+        <v>152</v>
+      </c>
+      <c r="H47" s="9"/>
+    </row>
+    <row r="48" ht="20.05" customHeight="1">
+      <c r="A48" s="11"/>
+      <c r="B48" s="7"/>
+      <c r="C48" t="s" s="8">
+        <v>58</v>
+      </c>
+      <c r="D48" t="s" s="8">
+        <v>64</v>
+      </c>
+      <c r="E48" t="s" s="8">
+        <v>65</v>
+      </c>
+      <c r="F48" t="s" s="8">
+        <v>66</v>
+      </c>
+      <c r="G48" s="12">
         <v>31172</v>
       </c>
-      <c r="H35" s="10"/>
-    </row>
-    <row r="36" ht="20.05" customHeight="1">
-      <c r="A36" s="11"/>
-      <c r="B36" s="9"/>
-      <c r="C36" t="s" s="8">
-        <v>69</v>
-      </c>
-      <c r="D36" t="s" s="8">
-        <v>115</v>
-      </c>
-      <c r="E36" t="s" s="8">
-        <v>116</v>
-      </c>
-      <c r="F36" t="s" s="8">
-        <v>117</v>
-      </c>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-    </row>
-    <row r="37" ht="20.05" customHeight="1">
-      <c r="A37" s="11"/>
-      <c r="B37" s="9"/>
-      <c r="C37" t="s" s="8">
-        <v>69</v>
-      </c>
-      <c r="D37" t="s" s="8">
-        <v>81</v>
-      </c>
-      <c r="E37" t="s" s="8">
-        <v>82</v>
-      </c>
-      <c r="F37" t="s" s="8">
-        <v>83</v>
-      </c>
-      <c r="G37" t="s" s="8">
-        <v>84</v>
-      </c>
-      <c r="H37" s="12">
+      <c r="H48" s="9"/>
+    </row>
+    <row r="49" ht="20.05" customHeight="1">
+      <c r="A49" s="11"/>
+      <c r="B49" s="7"/>
+      <c r="C49" t="s" s="8">
+        <v>58</v>
+      </c>
+      <c r="D49" t="s" s="8">
+        <v>153</v>
+      </c>
+      <c r="E49" t="s" s="8">
+        <v>154</v>
+      </c>
+      <c r="F49" t="s" s="8">
+        <v>155</v>
+      </c>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+    </row>
+    <row r="50" ht="20.05" customHeight="1">
+      <c r="A50" s="11"/>
+      <c r="B50" s="7"/>
+      <c r="C50" t="s" s="8">
+        <v>58</v>
+      </c>
+      <c r="D50" t="s" s="8">
+        <v>70</v>
+      </c>
+      <c r="E50" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="F50" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="G50" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="H50" s="12">
         <v>34734</v>
       </c>
     </row>
-    <row r="38" ht="20.05" customHeight="1">
-      <c r="A38" s="11"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-    </row>
-    <row r="39" ht="20.05" customHeight="1">
-      <c r="A39" s="11"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="10"/>
-      <c r="D39" t="s" s="8">
-        <v>118</v>
-      </c>
-      <c r="E39" t="s" s="8">
-        <v>119</v>
-      </c>
-      <c r="F39" t="s" s="8">
-        <v>120</v>
-      </c>
-      <c r="G39" t="s" s="8">
-        <v>121</v>
-      </c>
-      <c r="H39" s="10"/>
-    </row>
-    <row r="40" ht="20.05" customHeight="1">
-      <c r="A40" s="11"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-    </row>
-    <row r="41" ht="20.05" customHeight="1">
-      <c r="A41" s="11"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-    </row>
-    <row r="42" ht="20.05" customHeight="1">
-      <c r="A42" s="11"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
+    <row r="51" ht="20.05" customHeight="1">
+      <c r="A51" s="11"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+    </row>
+    <row r="52" ht="20.05" customHeight="1">
+      <c r="A52" s="11"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="9"/>
+      <c r="D52" t="s" s="8">
+        <v>156</v>
+      </c>
+      <c r="E52" t="s" s="8">
+        <v>157</v>
+      </c>
+      <c r="F52" t="s" s="8">
+        <v>158</v>
+      </c>
+      <c r="G52" t="s" s="8">
+        <v>159</v>
+      </c>
+      <c r="H52" s="9"/>
+    </row>
+    <row r="53" ht="20.05" customHeight="1">
+      <c r="A53" s="11"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+    </row>
+    <row r="54" ht="20.05" customHeight="1">
+      <c r="A54" s="11"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+    </row>
+    <row r="55" ht="20.05" customHeight="1">
+      <c r="A55" s="11"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" location="" tooltip="" display="myemail@mail.com"/>
-    <hyperlink ref="D3" r:id="rId2" location="" tooltip="" display="myemail2@mail.com"/>
-    <hyperlink ref="D4" r:id="rId3" location="" tooltip="" display="myemail3@mail.com"/>
-    <hyperlink ref="D6" r:id="rId4" location="" tooltip="" display="rsykes1234@mail.com"/>
-    <hyperlink ref="D7" r:id="rId5" location="" tooltip="" display="rsykes1234@mail.com"/>
-    <hyperlink ref="D8" r:id="rId6" location="" tooltip="" display="jdoe1234@mail.com"/>
-    <hyperlink ref="D9" r:id="rId7" location="" tooltip="" display="ihunter1234@mail.com"/>
-    <hyperlink ref="D10" r:id="rId8" location="" tooltip="" display="cgonzales1234@mail.com"/>
-    <hyperlink ref="D11" r:id="rId9" location="" tooltip="" display="rsykes1234@mail.com"/>
-    <hyperlink ref="D12" r:id="rId10" location="" tooltip="" display="dkelly1234@mail.com"/>
-    <hyperlink ref="D13" r:id="rId11" location="" tooltip="" display="rarnold1234@mail.com"/>
-    <hyperlink ref="D14" r:id="rId12" location="" tooltip="" display="mwalters1234@mail.com"/>
-    <hyperlink ref="D15" r:id="rId13" location="" tooltip="" display="TestSanboxx12@outlook.com"/>
-    <hyperlink ref="D16" r:id="rId14" location="" tooltip="" display="lukehatfield721@gmail.com"/>
-    <hyperlink ref="D17" r:id="rId15" location="" tooltip="" display="rossvance247@gmail.com"/>
-    <hyperlink ref="D18" r:id="rId16" location="" tooltip="" display="rossvance247@gmail.com"/>
-    <hyperlink ref="D19" r:id="rId17" location="" tooltip="" display="rossvance247@gmail.com"/>
-    <hyperlink ref="D20" r:id="rId18" location="" tooltip="" display="rossvance247@gmail.com"/>
-    <hyperlink ref="D21" r:id="rId19" location="" tooltip="" display="lukehatfield721@gmail.com"/>
-    <hyperlink ref="D22" r:id="rId20" location="" tooltip="" display="lukehatfield721@gmail.com"/>
-    <hyperlink ref="D23" r:id="rId21" location="" tooltip="" display="lukehatfield721@gmail.com"/>
-    <hyperlink ref="D24" r:id="rId22" location="" tooltip="" display="acarrol1234@mail.com"/>
-    <hyperlink ref="D25" r:id="rId23" location="" tooltip="" display="zarawalton254@gmail.com"/>
-    <hyperlink ref="D26" r:id="rId24" location="" tooltip="" display="amata1234@mail.com"/>
-    <hyperlink ref="D32" r:id="rId25" location="" tooltip="" display="twidel1234@mail.com"/>
-    <hyperlink ref="D33" r:id="rId26" location="" tooltip="" display="dkelly1234@mail.com"/>
-    <hyperlink ref="D34" r:id="rId27" location="" tooltip="" display="jkim1234@mail.com"/>
-    <hyperlink ref="D35" r:id="rId28" location="" tooltip="" display="lukehatfield721@gmail.com"/>
-    <hyperlink ref="D36" r:id="rId29" location="" tooltip="" display="rstone820@yahoo.com"/>
-    <hyperlink ref="D37" r:id="rId30" location="" tooltip="" display="rossvance247@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId2" location="" tooltip="" display="rsykes1234@mail.com"/>
+    <hyperlink ref="D5" r:id="rId3" location="" tooltip="" display="rsykes1234@mail.com"/>
+    <hyperlink ref="D7" r:id="rId4" location="" tooltip="" display="ihunter1234@mail.com"/>
+    <hyperlink ref="D8" r:id="rId5" location="" tooltip="" display="cgonzales1234@mail.com"/>
+    <hyperlink ref="D9" r:id="rId6" location="" tooltip="" display="rsykes1234@mail.com"/>
+    <hyperlink ref="D10" r:id="rId7" location="" tooltip="" display="dkelly1234@mail.com"/>
+    <hyperlink ref="D11" r:id="rId8" location="" tooltip="" display="rarnold1234@mail.com"/>
+    <hyperlink ref="D12" r:id="rId9" location="" tooltip="" display="mwalters1234@mail.com"/>
+    <hyperlink ref="D13" r:id="rId10" location="" tooltip="" display="TestSanboxx12@outlook.com"/>
+    <hyperlink ref="D14" r:id="rId11" location="" tooltip="" display="lukehatfield721@gmail.com"/>
+    <hyperlink ref="D15" r:id="rId12" location="" tooltip="" display="rossvance247@gmail.com"/>
+    <hyperlink ref="D16" r:id="rId13" location="" tooltip="" display="rossvance247@gmail.com"/>
+    <hyperlink ref="D17" r:id="rId14" location="" tooltip="" display="rossvance247@gmail.com"/>
+    <hyperlink ref="D18" r:id="rId15" location="" tooltip="" display="rossvance247@gmail.com"/>
+    <hyperlink ref="D19" r:id="rId16" location="" tooltip="" display="lukehatfield721@gmail.com"/>
+    <hyperlink ref="D20" r:id="rId17" location="" tooltip="" display="lukehatfield721@gmail.com"/>
+    <hyperlink ref="D21" r:id="rId18" location="" tooltip="" display="lukehatfield721@gmail.com"/>
+    <hyperlink ref="D22" r:id="rId19" location="" tooltip="" display="acarrol1234@mail.com"/>
+    <hyperlink ref="D23" r:id="rId20" location="" tooltip="" display="zarawalton254@gmail.com"/>
+    <hyperlink ref="D24" r:id="rId21" location="" tooltip="" display="amata1234@mail.com"/>
+    <hyperlink ref="D25" r:id="rId22" location="" tooltip="" display="psims1234@mail.com"/>
+    <hyperlink ref="D26" r:id="rId23" location="" tooltip="" display="lbyrne1234@mail.com"/>
+    <hyperlink ref="D27" r:id="rId24" location="" tooltip="" display="bcarter1234@mail.com"/>
+    <hyperlink ref="D28" r:id="rId25" location="" tooltip="" display="lbyrne1234@mail.com"/>
+    <hyperlink ref="D45" r:id="rId26" location="" tooltip="" display="twidel1234@mail.com"/>
+    <hyperlink ref="D46" r:id="rId27" location="" tooltip="" display="dkelly1234@mail.com"/>
+    <hyperlink ref="D47" r:id="rId28" location="" tooltip="" display="jkim1234@mail.com"/>
+    <hyperlink ref="D48" r:id="rId29" location="" tooltip="" display="lukehatfield721@gmail.com"/>
+    <hyperlink ref="D49" r:id="rId30" location="" tooltip="" display="rstone820@yahoo.com"/>
+    <hyperlink ref="D50" r:id="rId31" location="" tooltip="" display="rossvance247@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>